<commit_message>
nameId|String, spriteName|String 펫 신규 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Pet.xlsx
+++ b/Excel/Pet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C06C8B-B469-4F49-BA0D-13C77C85E6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C77A14B-5F0F-47C1-B195-33C08FF1AA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2CD979F8-641A-489B-AD59-45F7500B59B8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Pet_0002</t>
   </si>
@@ -79,6 +79,33 @@
   </si>
   <si>
     <t>TamporaA</t>
+  </si>
+  <si>
+    <t>nameId|String</t>
+  </si>
+  <si>
+    <t>spriteName|String</t>
+  </si>
+  <si>
+    <t>PetName_0001</t>
+  </si>
+  <si>
+    <t>PetPortrait_0001</t>
+  </si>
+  <si>
+    <t>PetName_0002</t>
+  </si>
+  <si>
+    <t>PetName_0003</t>
+  </si>
+  <si>
+    <t>PetName_0004</t>
+  </si>
+  <si>
+    <t>PetName_0005</t>
+  </si>
+  <si>
+    <t>PetName_0006</t>
   </si>
 </sst>
 </file>
@@ -442,155 +469,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34D833B-1531-4D0A-8119-5FB3C5757C64}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="1" max="2" width="12.125" customWidth="1"/>
+    <col min="5" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>23</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>1</v>
       </c>
     </row>

</xml_diff>